<commit_message>
Customize MCGLT to hit 1.5 target
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="840" windowWidth="16680" windowHeight="16725"/>
+    <workbookView xWindow="3675" yWindow="840" windowWidth="16680" windowHeight="16725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="6" r:id="rId1"/>
@@ -843,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1556,8 +1556,8 @@
   </sheetPr>
   <dimension ref="A1:AW32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1592,11 +1592,11 @@
         <v>118</v>
       </c>
       <c r="C2" s="13">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="13">
         <f>C2</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.45">
@@ -1619,11 +1619,11 @@
         <v>118</v>
       </c>
       <c r="C4" s="13">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D4" s="13">
         <f>C4</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.45">
@@ -1646,11 +1646,11 @@
         <v>118</v>
       </c>
       <c r="C6" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D6" s="11">
         <f>C6</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.45">
@@ -1673,11 +1673,11 @@
         <v>118</v>
       </c>
       <c r="C8" s="13">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D8" s="11">
         <f>C8</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1715,11 +1715,11 @@
         <v>118</v>
       </c>
       <c r="C10" s="5">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D10" s="13">
         <f>C10</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1782,11 +1782,11 @@
         <v>118</v>
       </c>
       <c r="C12" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D12" s="13">
         <f>C12</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
@@ -1876,11 +1876,11 @@
         <v>118</v>
       </c>
       <c r="C14" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D14" s="11">
         <f>C14</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.45">
@@ -1903,11 +1903,11 @@
         <v>118</v>
       </c>
       <c r="C16" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D16" s="11">
         <f>C16</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1930,11 +1930,11 @@
         <v>118</v>
       </c>
       <c r="C18" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D18" s="11">
         <f>C18</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -1957,11 +1957,11 @@
         <v>118</v>
       </c>
       <c r="C20" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D20" s="11">
         <f>C20</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1984,11 +1984,11 @@
         <v>118</v>
       </c>
       <c r="C22" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D22" s="11">
         <f>C22</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -2011,11 +2011,11 @@
         <v>118</v>
       </c>
       <c r="C24" s="13">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D24" s="5">
         <f>C24</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -2069,7 +2069,7 @@
         <v>118</v>
       </c>
       <c r="C28" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D28" s="11">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>118</v>
       </c>
       <c r="C30" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D30" s="11">
         <v>0</v>
@@ -2121,11 +2121,11 @@
         <v>118</v>
       </c>
       <c r="C32" s="11">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="D32" s="11">
         <f>C32</f>
-        <v>500</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>